<commit_message>
changes to background text and images
</commit_message>
<xml_diff>
--- a/docs/classification_example.xlsx
+++ b/docs/classification_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akileshramakrishna/UVA /DSPG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/digvijayghotane/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46BEDA74-69B7-B341-A492-3443A741D787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C30B858-B674-C342-9B86-F6CBF26FFA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{1D5AAAD3-319E-6E4B-95C3-FBE6BD187DCC}"/>
+    <workbookView xWindow="14420" yWindow="500" windowWidth="14380" windowHeight="16240" xr2:uid="{1D5AAAD3-319E-6E4B-95C3-FBE6BD187DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>More efficient diagnostics with proprietary AI machine-learning technology</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -510,14 +513,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1F3E55-1278-B045-886E-53578179F4D1}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" s="5" t="s">
         <v>20</v>
       </c>

</xml_diff>